<commit_message>
Week 14: Release 0.2
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c9-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c9-tables.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B72D40-3189-4193-8784-03F2B150BE6B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B68F66B-8D0F-4DA6-B889-FC89F9B98EEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{2D9CA2C9-3410-4B25-85EA-9E0DEF3AF67E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{2D9CA2C9-3410-4B25-85EA-9E0DEF3AF67E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Tutorials Q3-5" sheetId="2" r:id="rId2"/>
     <sheet name="TQ6-END" sheetId="3" r:id="rId3"/>
+    <sheet name="T9Q1" sheetId="4" r:id="rId4"/>
+    <sheet name="T9Q2" sheetId="5" r:id="rId5"/>
+    <sheet name="T9Q3" sheetId="6" r:id="rId6"/>
+    <sheet name="T9Q4" sheetId="7" r:id="rId7"/>
+    <sheet name="T9Q5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
   <si>
     <t>C9: Index Number Tables</t>
   </si>
@@ -372,6 +377,156 @@
   </si>
   <si>
     <t>Real expenditure</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>Fixed base relatives</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Chain base relatives</t>
+  </si>
+  <si>
+    <t>N.A</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price in year 1 </t>
+  </si>
+  <si>
+    <t>Price in year 2</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>(a)</t>
+  </si>
+  <si>
+    <t>(b)</t>
+  </si>
+  <si>
+    <t>(d)</t>
+  </si>
+  <si>
+    <t>W*PRI</t>
+  </si>
+  <si>
+    <t>e)</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>W*P0</t>
+  </si>
+  <si>
+    <t>W*P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production ( in thousands units ) </t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>Q1/Q0*100</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <t>Price, W</t>
+  </si>
+  <si>
+    <t>W*Q1/Q0*100</t>
+  </si>
+  <si>
+    <t>Durable House Good</t>
+  </si>
+  <si>
+    <t>Price Relative</t>
+  </si>
+  <si>
+    <t>PR*W</t>
+  </si>
+  <si>
+    <t>Price of Living Index</t>
+  </si>
+  <si>
+    <t>Price in 2005</t>
+  </si>
+  <si>
+    <t>Quantity in 2005</t>
+  </si>
+  <si>
+    <t>Price in 2010</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>P1/P0*100</t>
+  </si>
+  <si>
+    <t>P1Q1/P0Q0*100</t>
+  </si>
+  <si>
+    <t>P0Q0</t>
+  </si>
+  <si>
+    <t>P0Q1</t>
+  </si>
+  <si>
+    <t>P1Q1</t>
+  </si>
+  <si>
+    <t>P1Q0</t>
+  </si>
+  <si>
+    <t>f)</t>
+  </si>
+  <si>
+    <t>g)</t>
+  </si>
+  <si>
+    <t>h)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +566,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -557,11 +712,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -576,6 +768,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,15 +785,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1115,26 +1320,26 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1145,7 +1350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1153,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1991</v>
       </c>
@@ -1161,7 +1366,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>1992</v>
       </c>
@@ -1169,7 +1374,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>1993</v>
       </c>
@@ -1177,27 +1382,27 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="16">
         <v>1999</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="14">
+      <c r="D13" s="17"/>
+      <c r="E13" s="16">
         <v>2002</v>
       </c>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="15"/>
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
@@ -1228,7 +1433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1261,41 +1466,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0386C5-CD65-45D4-97F7-F01FB68CBEA1}">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="20">
         <v>2007</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="3">
         <v>2007</v>
       </c>
@@ -1309,14 +1514,14 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3">
         <v>62</v>
       </c>
@@ -1330,14 +1535,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="20">
         <v>3</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="3">
         <v>138</v>
       </c>
@@ -1351,14 +1556,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="20">
         <v>0.5</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="3">
         <v>500</v>
       </c>
@@ -1372,14 +1577,14 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="20">
         <v>4.5</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="3">
         <v>10</v>
       </c>
@@ -1393,23 +1598,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>F4/D4*100</f>
         <v>106.45161290322579</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>2007</v>
       </c>
@@ -1417,7 +1622,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>62</v>
       </c>
@@ -1425,7 +1630,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>138</v>
       </c>
@@ -1433,7 +1638,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>500</v>
       </c>
@@ -1441,7 +1646,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>10</v>
       </c>
@@ -1449,7 +1654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1462,7 +1667,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1471,12 +1676,12 @@
         <v>103.52112676056338</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>2007</v>
       </c>
@@ -1487,7 +1692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>62</v>
       </c>
@@ -1499,7 +1704,7 @@
         <v>106.45161290322579</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>138</v>
       </c>
@@ -1511,7 +1716,7 @@
         <v>79.710144927536234</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>500</v>
       </c>
@@ -1523,7 +1728,7 @@
         <v>115.99999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>10</v>
       </c>
@@ -1535,7 +1740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1544,28 +1749,28 @@
         <v>100.54043945769051</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20" t="s">
+      <c r="C37" s="20"/>
+      <c r="D37" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B38" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="3">
         <v>2007</v>
       </c>
@@ -1579,11 +1784,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="19">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="20">
         <v>2</v>
       </c>
-      <c r="C39" s="19"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="3">
         <v>62</v>
       </c>
@@ -1599,11 +1804,11 @@
         <v>212.90322580645159</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="19">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="20">
         <v>3</v>
       </c>
-      <c r="C40" s="19"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="3">
         <v>138</v>
       </c>
@@ -1619,11 +1824,11 @@
         <v>239.13043478260869</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="19">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="20">
         <v>0.5</v>
       </c>
-      <c r="C41" s="19"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="3">
         <v>500</v>
       </c>
@@ -1639,11 +1844,11 @@
         <v>57.999999999999993</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="20">
         <v>4.5</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="3">
         <v>10</v>
       </c>
@@ -1659,7 +1864,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F43" t="s">
         <v>21</v>
       </c>
@@ -1668,7 +1873,7 @@
         <v>960.03366058906022</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1677,28 +1882,28 @@
         <v>96.003366058906025</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="19" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="20" t="s">
+      <c r="C49" s="20"/>
+      <c r="D49" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="19" t="s">
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="19"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="3">
         <v>2007</v>
       </c>
@@ -1712,11 +1917,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="19">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B51" s="20">
         <v>2</v>
       </c>
-      <c r="C51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="3">
         <v>62</v>
       </c>
@@ -1732,11 +1937,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="19">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B52" s="20">
         <v>3</v>
       </c>
-      <c r="C52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="3">
         <v>138</v>
       </c>
@@ -1752,11 +1957,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="19">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="20">
         <v>0.5</v>
       </c>
-      <c r="C53" s="19"/>
+      <c r="C53" s="20"/>
       <c r="D53" s="3">
         <v>500</v>
       </c>
@@ -1772,11 +1977,11 @@
         <v>400</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="19">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="20">
         <v>4.5</v>
       </c>
-      <c r="C54" s="19"/>
+      <c r="C54" s="20"/>
       <c r="D54" s="3">
         <v>10</v>
       </c>
@@ -1792,7 +1997,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E55" t="s">
         <v>21</v>
       </c>
@@ -1805,7 +2010,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1814,16 +2019,16 @@
         <v>103.84153661464586</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B60" s="18"/>
+      <c r="B60" s="22"/>
       <c r="C60" t="s">
         <v>35</v>
       </c>
@@ -1843,11 +2048,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="18"/>
+      <c r="B61" s="22"/>
       <c r="C61">
         <v>103.4</v>
       </c>
@@ -1867,11 +2072,11 @@
         <v>107.2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="18"/>
+      <c r="B62" s="22"/>
       <c r="C62">
         <v>25</v>
       </c>
@@ -1891,11 +2096,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="17"/>
+      <c r="B63" s="21"/>
       <c r="C63">
         <f>C61*C62</f>
         <v>2585</v>
@@ -1921,12 +2126,12 @@
         <v>857.6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>45</v>
       </c>
@@ -1935,12 +2140,12 @@
         <v>107.32000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -1957,7 +2162,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -1974,7 +2179,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -1991,50 +2196,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <f>D72/B72*100</f>
         <v>114.28571428571428</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <f>E73/C73*100</f>
         <v>87.654320987654316</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <f>(D72*E72)/(C72*B72)*100</f>
         <v>144.26229508196721</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -2057,7 +2262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -2082,7 +2287,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +2312,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E89" t="s">
         <v>58</v>
       </c>
@@ -2120,7 +2325,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>59</v>
       </c>
@@ -2129,12 +2334,12 @@
         <v>126.80288461538463</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2385,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2408,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E98" t="s">
         <v>58</v>
       </c>
@@ -2214,7 +2419,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -2223,12 +2428,12 @@
         <v>124.496644295302</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -2251,7 +2456,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -2276,7 +2481,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -2301,7 +2506,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E107" t="s">
         <v>58</v>
       </c>
@@ -2314,7 +2519,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>67</v>
       </c>
@@ -2323,12 +2528,12 @@
         <v>107.45192307692308</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -2351,7 +2556,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>14</v>
       </c>
@@ -2376,7 +2581,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>15</v>
       </c>
@@ -2401,7 +2606,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E117" t="s">
         <v>58</v>
       </c>
@@ -2414,7 +2619,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>68</v>
       </c>
@@ -2423,12 +2628,12 @@
         <v>105.49763033175354</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -2451,7 +2656,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -2476,7 +2681,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>15</v>
       </c>
@@ -2501,7 +2706,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E126" t="s">
         <v>58</v>
       </c>
@@ -2514,7 +2719,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>71</v>
       </c>
@@ -2525,20 +2730,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
     <mergeCell ref="D37:G37"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="D49:G49"/>
@@ -2550,6 +2741,20 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:B61"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2560,28 +2765,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94F07DE-6747-446E-B281-4D3881C052C1}">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -2598,7 +2803,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2615,7 +2820,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2632,7 +2837,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2649,17 +2854,17 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2668,12 +2873,12 @@
         <v>118.83116883116884</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2682,12 +2887,12 @@
         <v>89.583333333333343</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2696,7 +2901,7 @@
         <v>104.30879712746859</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -2705,22 +2910,22 @@
         <v>113.72549019607843</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="23"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -2743,7 +2948,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2768,7 +2973,7 @@
         <v>114.85714285714286</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2793,7 +2998,7 @@
         <v>143.75</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2818,7 +3023,7 @@
         <v>89.583333333333343</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -2827,7 +3032,7 @@
         <v>108.79046492706198</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -2836,22 +3041,22 @@
         <v>116.06349206349209</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2880,7 +3085,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2913,7 +3118,7 @@
         <v>3678.3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2946,7 +3151,7 @@
         <v>685.4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +3184,7 @@
         <v>1070.7</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F40" s="10">
         <f>SUM(F37:F39)</f>
         <v>4426.2000000000007</v>
@@ -2997,7 +3202,7 @@
         <v>5434.4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -3006,7 +3211,7 @@
         <v>110.12832678143778</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -3015,7 +3220,7 @@
         <v>111.6718724313661</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -3024,22 +3229,22 @@
         <v>110.89741412411976</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B47" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21" t="s">
+      <c r="C47" s="23"/>
+      <c r="D47" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -3068,7 +3273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3101,7 +3306,7 @@
         <v>3678.3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3134,7 +3339,7 @@
         <v>685.4</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -3167,7 +3372,7 @@
         <v>1070.7</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F52" s="10">
         <f>SUM(F49:F51)</f>
         <v>4426.2000000000007</v>
@@ -3185,7 +3390,7 @@
         <v>5434.4</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -3194,7 +3399,7 @@
         <v>109.94532556142964</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -3203,7 +3408,7 @@
         <v>111.48630628782439</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -3212,12 +3417,12 @@
         <v>110.71313490483463</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -3226,12 +3431,12 @@
         <v>122.77800370520985</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -3257,7 +3462,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -3283,7 +3488,7 @@
         <v>151.16</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -3309,7 +3514,7 @@
         <v>156.22999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>103</v>
       </c>
@@ -3342,49 +3547,49 @@
         <v>132.04022988505747</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <f>(64000+11800)/(64000)*100</f>
         <v>118.4375</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <f>150/120*100</f>
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -3410,7 +3615,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>110</v>
       </c>
@@ -3436,7 +3641,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>111</v>
       </c>
@@ -3462,7 +3667,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>112</v>
       </c>
@@ -3508,4 +3713,1161 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7C6113-8C86-496B-B722-45A5A30B9DCA}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>216.9</v>
+      </c>
+      <c r="C3">
+        <v>225.1</v>
+      </c>
+      <c r="D3">
+        <v>234.6</v>
+      </c>
+      <c r="E3">
+        <v>237.2</v>
+      </c>
+      <c r="F3">
+        <v>235.2</v>
+      </c>
+      <c r="G3">
+        <v>230.1</v>
+      </c>
+      <c r="H3">
+        <v>224.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f>B3/216.9*100</f>
+        <v>100</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:H5" si="0">C3/216.9*100</f>
+        <v>103.78054402950667</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>108.16044260027662</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" si="0"/>
+        <v>109.35915168280313</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>108.43706777316736</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>106.08575380359613</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="0"/>
+        <v>103.45781466113418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7">
+        <f>C3/B3*100</f>
+        <v>103.78054402950667</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" ref="D7:H7" si="1">D3/C3*100</f>
+        <v>104.22034651266104</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="1"/>
+        <v>101.1082693947144</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="1"/>
+        <v>99.156829679595276</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="1"/>
+        <v>97.831632653061234</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="1"/>
+        <v>97.522816166883956</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873C39CD-FFB7-4170-8E11-52D2EE2ECDC2}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="4" max="5" width="14.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>215</v>
+      </c>
+      <c r="E3">
+        <v>210</v>
+      </c>
+      <c r="F3" s="12">
+        <f>E3/D3*100</f>
+        <v>97.674418604651152</v>
+      </c>
+      <c r="G3">
+        <f>C3*F3</f>
+        <v>488.37209302325573</v>
+      </c>
+      <c r="H3">
+        <f>C3*D3</f>
+        <v>1075</v>
+      </c>
+      <c r="I3">
+        <f>C3*E3</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>250</v>
+      </c>
+      <c r="E4">
+        <v>275</v>
+      </c>
+      <c r="F4" s="12">
+        <f>E4/D4*100</f>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="G4">
+        <f>C4*F4</f>
+        <v>1320.0000000000002</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" ref="H4:H6" si="0">C4*D4</f>
+        <v>3000</v>
+      </c>
+      <c r="I4" s="12">
+        <f t="shared" ref="I4:I6" si="1">C4*E4</f>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1100</v>
+      </c>
+      <c r="E5">
+        <v>1300</v>
+      </c>
+      <c r="F5" s="12">
+        <f>E5/D5*100</f>
+        <v>118.18181818181819</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:G7" si="2">C5*F5</f>
+        <v>236.36363636363637</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>950</v>
+      </c>
+      <c r="E6">
+        <v>950</v>
+      </c>
+      <c r="F6" s="12">
+        <f>E6/D6*100</f>
+        <v>100</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="0"/>
+        <v>7600</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="1"/>
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D3:D6)</f>
+        <v>2515</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E3:E6)</f>
+        <v>2735</v>
+      </c>
+      <c r="F7">
+        <f>SUM(F3:F6)</f>
+        <v>425.85623678646937</v>
+      </c>
+      <c r="G7" s="12">
+        <f>SUM(G3:G6)</f>
+        <v>2844.7357293868922</v>
+      </c>
+      <c r="H7">
+        <f>SUM(H3:H6)</f>
+        <v>13875</v>
+      </c>
+      <c r="I7">
+        <f>SUM(I3:I6)</f>
+        <v>14550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <f>E5/D5*100</f>
+        <v>118.18181818181819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10">
+        <f>E7/D7*100</f>
+        <v>108.74751491053678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <f>1/4*SUM(F3:F6)</f>
+        <v>106.46405919661734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12">
+        <f>1/C7*G7</f>
+        <v>105.3605825698849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13">
+        <f>I7/H7*100</f>
+        <v>104.86486486486486</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9CB95B-D637-4ADB-8911-B7AE77791B71}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2007</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2007</v>
+      </c>
+      <c r="D2" s="13">
+        <v>2008</v>
+      </c>
+      <c r="E2" s="13">
+        <v>2009</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
+        <v>62</v>
+      </c>
+      <c r="D3" s="13">
+        <v>65</v>
+      </c>
+      <c r="E3" s="13">
+        <v>66</v>
+      </c>
+      <c r="F3" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13">
+        <v>138</v>
+      </c>
+      <c r="D4" s="13">
+        <v>120</v>
+      </c>
+      <c r="E4" s="13">
+        <v>110</v>
+      </c>
+      <c r="F4" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="13">
+        <v>500</v>
+      </c>
+      <c r="D5" s="13">
+        <v>540</v>
+      </c>
+      <c r="E5" s="13">
+        <v>580</v>
+      </c>
+      <c r="F5" s="13">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="13">
+        <v>4.5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>10</v>
+      </c>
+      <c r="D6" s="13">
+        <v>10</v>
+      </c>
+      <c r="E6" s="13">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v>2717</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9">
+        <f>E3/C3*100</f>
+        <v>106.45161290322579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10">
+        <f>D7/C7*100</f>
+        <v>100.95693779904306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2007</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2009</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2010</v>
+      </c>
+      <c r="G11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13">
+        <v>62</v>
+      </c>
+      <c r="E12" s="13">
+        <v>66</v>
+      </c>
+      <c r="F12" s="13">
+        <v>90</v>
+      </c>
+      <c r="G12">
+        <f>E12/D12*100</f>
+        <v>106.45161290322579</v>
+      </c>
+      <c r="H12">
+        <f>C12*G12</f>
+        <v>212.90322580645159</v>
+      </c>
+      <c r="I12">
+        <f>C12*D12</f>
+        <v>124</v>
+      </c>
+      <c r="J12">
+        <f>C12*F12</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="12">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13">
+        <v>138</v>
+      </c>
+      <c r="E13" s="13">
+        <v>110</v>
+      </c>
+      <c r="F13" s="13">
+        <v>80</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" ref="G13:G15" si="0">E13/D13*100</f>
+        <v>79.710144927536234</v>
+      </c>
+      <c r="H13" s="12">
+        <f>C13*G13</f>
+        <v>239.13043478260869</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" ref="I13:I15" si="1">C13*D13</f>
+        <v>414</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" ref="J13:J15" si="2">C13*F13</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="13">
+        <v>500</v>
+      </c>
+      <c r="E14" s="13">
+        <v>580</v>
+      </c>
+      <c r="F14" s="13">
+        <v>800</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="0"/>
+        <v>115.99999999999999</v>
+      </c>
+      <c r="H14" s="12">
+        <f>C14*G14</f>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="D15" s="13">
+        <v>10</v>
+      </c>
+      <c r="E15" s="13">
+        <v>10</v>
+      </c>
+      <c r="F15" s="13">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H15" s="12">
+        <f>C15*G15</f>
+        <v>450</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J15" s="12">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C12:C15)</f>
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <f>SUM(G12:G15)</f>
+        <v>402.16175783076204</v>
+      </c>
+      <c r="H16" s="12">
+        <f>SUM(H12:H15)</f>
+        <v>960.03366058906022</v>
+      </c>
+      <c r="I16">
+        <f>SUM(I12:I15)</f>
+        <v>833</v>
+      </c>
+      <c r="J16" s="12">
+        <f>SUM(J12:J15)</f>
+        <v>865</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <f>1/4*G16</f>
+        <v>100.54043945769051</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19">
+        <f>1/C16*H16</f>
+        <v>96.003366058906025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20">
+        <f>J16/I16*100</f>
+        <v>103.84153661464586</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A133456B-204C-43FC-8AE0-A29BCA9839A5}">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3">
+        <v>103.4</v>
+      </c>
+      <c r="C3">
+        <v>112.5</v>
+      </c>
+      <c r="D3">
+        <v>111.2</v>
+      </c>
+      <c r="E3">
+        <v>115.3</v>
+      </c>
+      <c r="F3">
+        <v>100.6</v>
+      </c>
+      <c r="G3">
+        <v>107.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <f>SUM(B4:G4)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5">
+        <f>B3*B4</f>
+        <v>2585</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" ref="C5:G5" si="0">C3*C4</f>
+        <v>1350</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>1223.2</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" si="0"/>
+        <v>691.8</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>804.8</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>857.6</v>
+      </c>
+      <c r="H5">
+        <f>SUM(B5:G5)</f>
+        <v>7512.4000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7">
+        <f>H5/H4</f>
+        <v>107.32000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E60D5A-D9D9-4CDD-92D9-972097F0F7F5}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>77</v>
+      </c>
+      <c r="G2">
+        <f>E2/C2*100</f>
+        <v>114.28571428571428</v>
+      </c>
+      <c r="H2" s="12">
+        <f>F2/D2*100</f>
+        <v>126.22950819672131</v>
+      </c>
+      <c r="I2">
+        <f>E2*F2/(D2*C2)*100</f>
+        <v>144.26229508196721</v>
+      </c>
+      <c r="J2">
+        <f>C2*D2</f>
+        <v>427</v>
+      </c>
+      <c r="K2">
+        <f>C2*F2</f>
+        <v>539</v>
+      </c>
+      <c r="L2">
+        <f>E2*D2</f>
+        <v>488</v>
+      </c>
+      <c r="M2">
+        <f>E2*F2</f>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>81</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>71</v>
+      </c>
+      <c r="G3" s="12">
+        <f>E3/C3</f>
+        <v>1.4</v>
+      </c>
+      <c r="H3">
+        <f>F3/D3*100</f>
+        <v>87.654320987654316</v>
+      </c>
+      <c r="I3" s="12">
+        <f>E3*F3/(D3*C3)*100</f>
+        <v>122.71604938271605</v>
+      </c>
+      <c r="J3" s="12">
+        <f>C3*D3</f>
+        <v>405</v>
+      </c>
+      <c r="K3" s="12">
+        <f>C3*F3</f>
+        <v>355</v>
+      </c>
+      <c r="L3" s="12">
+        <f>E3*D3</f>
+        <v>567</v>
+      </c>
+      <c r="M3" s="12">
+        <f>E3*F3</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="12">
+        <f>SUM(C2:C3)</f>
+        <v>12</v>
+      </c>
+      <c r="D4" s="12">
+        <f t="shared" ref="D4:M4" si="0">SUM(D2:D3)</f>
+        <v>142</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>115.68571428571428</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" si="0"/>
+        <v>213.88382918437563</v>
+      </c>
+      <c r="I4" s="12">
+        <f t="shared" si="0"/>
+        <v>266.97834446468323</v>
+      </c>
+      <c r="J4" s="12">
+        <f t="shared" si="0"/>
+        <v>832</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" si="0"/>
+        <v>894</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" si="0"/>
+        <v>1055</v>
+      </c>
+      <c r="M4" s="12">
+        <f t="shared" si="0"/>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5">
+        <f>G2</f>
+        <v>114.28571428571428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6">
+        <f>H3</f>
+        <v>87.654320987654316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7">
+        <f>I2</f>
+        <v>144.26229508196721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8">
+        <f>L4/J4*100</f>
+        <v>126.80288461538463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9">
+        <f>M4/K4*100</f>
+        <v>124.496644295302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <f>K4/J4*100</f>
+        <v>107.45192307692308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11">
+        <f>M4/L4*100</f>
+        <v>105.49763033175354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12">
+        <f>M4/J4*100</f>
+        <v>133.77403846153845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>